<commit_message>
fixed hysplits.xlsx to INP(T) data, fixed Niemand param to cover all data in contour3, fixed graph in hysplits.py to give viewable legend size
</commit_message>
<xml_diff>
--- a/hysplits.xlsx
+++ b/hysplits.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eardo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eardo\Desktop\Farmscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="14">
   <si>
     <t>D1</t>
   </si>
@@ -75,10 +75,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -103,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -112,6 +118,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -397,7 +406,7 @@
   <dimension ref="A1:G1048538"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -439,7 +448,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -453,7 +462,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -467,7 +476,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -481,7 +490,7 @@
         <v>0.625</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -539,6 +548,9 @@
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -553,6 +565,9 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -567,6 +582,9 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -581,6 +599,9 @@
         <v>0.625</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -787,10 +808,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>8</v>
@@ -807,10 +828,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>8</v>
@@ -827,10 +848,10 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>8</v>
@@ -847,10 +868,10 @@
         <v>0.625</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>8</v>
@@ -1250,11 +1271,11 @@
       <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>7</v>
+      <c r="C54" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1264,11 +1285,11 @@
       <c r="B55" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>7</v>
+      <c r="C55" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1278,11 +1299,11 @@
       <c r="B56" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>7</v>
+      <c r="C56" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>8</v>
@@ -1295,8 +1316,8 @@
       <c r="B57" s="2">
         <v>0.625</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>9</v>
+      <c r="C57" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>7</v>
@@ -1315,6 +1336,9 @@
       <c r="C58" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D58" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F58" s="1" t="s">
         <v>8</v>
       </c>
@@ -1329,6 +1353,9 @@
       <c r="C59" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D59" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F59" s="1" t="s">
         <v>8</v>
       </c>
@@ -1343,6 +1370,9 @@
       <c r="C60" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D60" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F60" s="1" t="s">
         <v>8</v>
       </c>
@@ -1357,6 +1387,9 @@
       <c r="C61" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D61" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F61" s="1" t="s">
         <v>8</v>
       </c>
@@ -1369,7 +1402,7 @@
         <v>5</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>7</v>
@@ -1389,7 +1422,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>7</v>
@@ -1409,7 +1442,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>7</v>
@@ -1429,7 +1462,7 @@
         <v>0.625</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>7</v>
@@ -1679,6 +1712,9 @@
       <c r="C78" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D78" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="G78" s="1" t="s">
         <v>8</v>
       </c>
@@ -1693,6 +1729,9 @@
       <c r="C79" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D79" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="G79" s="1" t="s">
         <v>8</v>
       </c>
@@ -1707,6 +1746,9 @@
       <c r="C80" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D80" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="G80" s="1" t="s">
         <v>8</v>
       </c>
@@ -1721,6 +1763,9 @@
       <c r="C81" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D81" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="G81" s="1" t="s">
         <v>8</v>
       </c>
@@ -1775,7 +1820,7 @@
         <v>0.625</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>7</v>
@@ -1795,7 +1840,7 @@
         <v>0.5</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>7</v>
@@ -1812,7 +1857,7 @@
         <v>11</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>7</v>
@@ -1829,7 +1874,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>7</v>
@@ -1846,7 +1891,7 @@
         <v>0.625</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>7</v>
@@ -1863,7 +1908,7 @@
         <v>0.5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>8</v>
@@ -1877,7 +1922,7 @@
         <v>11</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>8</v>
@@ -1951,5 +1996,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added modifications so that hysplits can now be plotted together with trajectories for figure 3
</commit_message>
<xml_diff>
--- a/hysplits.xlsx
+++ b/hysplits.xlsx
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1048538"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -448,7 +448,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -462,7 +462,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -476,7 +476,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -490,7 +490,7 @@
         <v>0.625</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -515,7 +515,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -526,7 +526,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -537,7 +537,7 @@
         <v>0.625</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -565,7 +565,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
@@ -582,7 +582,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
@@ -599,7 +599,7 @@
         <v>0.625</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>7</v>
@@ -1272,7 +1272,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>7</v>
@@ -1286,7 +1286,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>7</v>
@@ -1300,7 +1300,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>7</v>
@@ -1317,7 +1317,7 @@
         <v>0.625</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>7</v>
@@ -1840,7 +1840,7 @@
         <v>0.5</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>7</v>
@@ -1857,7 +1857,7 @@
         <v>11</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>7</v>
@@ -1874,7 +1874,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>7</v>
@@ -1891,7 +1891,7 @@
         <v>0.625</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>7</v>
@@ -1908,7 +1908,7 @@
         <v>0.5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>8</v>
@@ -1922,7 +1922,7 @@
         <v>11</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>8</v>
@@ -1995,6 +1995,9 @@
       <c r="B1048538" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="A2:G96">
+    <sortCondition ref="A2:A96"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>